<commit_message>
GoodInfo_v2 - 2021-12-27 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,20 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2021-12-27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.25%</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2021-12-30 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,20 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021-12-30</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-0.56%</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-03 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,28 +544,51 @@
           <t>2021-12-30</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>56348.0</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-318.0</t>
-        </is>
+      <c r="B6" t="n">
+        <v>56348</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-318</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>-0.56%</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-363.0</t>
-        </is>
+      <c r="E6" t="n">
+        <v>-363</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-01-03</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>56348.0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-1065.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-1.89%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-04 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,28 +567,51 @@
           <t>2022-01-03</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>56348.0</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-1065.0</t>
-        </is>
+      <c r="B7" t="n">
+        <v>56348</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1065</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>-1.89%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E7" t="n">
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-01-04</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>56348.0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-1090.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-1.93%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-05 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,28 +590,51 @@
           <t>2022-01-04</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>56348.0</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-1090.0</t>
-        </is>
+      <c r="B8" t="n">
+        <v>56348</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1090</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>-1.93%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E8" t="n">
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-01-05</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>56348.0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>-2706.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-4.8%</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-06 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,28 +613,51 @@
           <t>2022-01-05</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>56348.0</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>-2706.0</t>
-        </is>
+      <c r="B9" t="n">
+        <v>56348</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2706</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>-4.8%</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E9" t="n">
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2022-01-06</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>56348.0</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-2074.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-3.68%</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-11 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,28 +636,51 @@
           <t>2022-01-06</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>56348.0</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>-2074.0</t>
-        </is>
+      <c r="B10" t="n">
+        <v>56348</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2074</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>-3.68%</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E10" t="n">
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022-01-11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>56308.0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-1656.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>-2.94%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-3264.0</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-12 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,28 +659,51 @@
           <t>2022-01-11</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>56308.0</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>-1656.0</t>
-        </is>
+      <c r="B11" t="n">
+        <v>56308</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1656</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>-2.94%</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>-3264.0</t>
-        </is>
+      <c r="E11" t="n">
+        <v>-3264</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022-01-12</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>56308.0</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>-935.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>-1.66%</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-18 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -728,28 +728,51 @@
           <t>2022-01-17</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>54446.0</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>-74.0</t>
-        </is>
+      <c r="B14" t="n">
+        <v>54446</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-74</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>-0.14%</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>-2041.0</t>
-        </is>
+      <c r="E14" t="n">
+        <v>-2041</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2022-01-18</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>54446.0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>252.0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.46%</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-19 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -751,28 +751,51 @@
           <t>2022-01-18</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>54446.0</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>252.0</t>
-        </is>
+      <c r="B15" t="n">
+        <v>54446</v>
+      </c>
+      <c r="C15" t="n">
+        <v>252</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>0.46%</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E15" t="n">
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2022-01-19</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>54446.0</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>175.0</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.32%</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-20 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -774,28 +774,51 @@
           <t>2022-01-19</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>54446.0</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>175.0</t>
-        </is>
+      <c r="B16" t="n">
+        <v>54446</v>
+      </c>
+      <c r="C16" t="n">
+        <v>175</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>0.32%</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2022-01-20</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>54446.0</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>706.0</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1.3%</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GoodInfo_v2 - 2022-01-21 未完成
</commit_message>
<xml_diff>
--- a/profit.xlsx
+++ b/profit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,28 +797,39 @@
           <t>2022-01-20</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>54446.0</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>706.0</t>
-        </is>
+      <c r="B17" t="n">
+        <v>54446</v>
+      </c>
+      <c r="C17" t="n">
+        <v>706</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>1.3%</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E17" t="n">
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2022-01-21</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-2272.0</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>